<commit_message>
final changes on burndowns
</commit_message>
<xml_diff>
--- a/ncis-issue-milestones.xlsx
+++ b/ncis-issue-milestones.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD9E68DA-7842-47A5-BD19-32A4D6CEB75E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FA4AC3B-8E54-4E16-9690-90019EE0B130}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -863,6 +863,7 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="2119071216"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -920,6 +921,7 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="107205648"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
@@ -1719,6 +1721,7 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="2119080784"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -1776,6 +1779,7 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="104992912"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>

</xml_diff>